<commit_message>
Updated keywords keyboard shortcut
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/keyboard_shortcut_test_data.xlsx
+++ b/TestData/Web_POS/Billing/keyboard_shortcut_test_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115" count="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="116" count="492">
   <si>
     <t>TC_Id</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>KB_30</t>
+  </si>
+  <si>
+    <t>Return</t>
   </si>
 </sst>
 </file>
@@ -389,12 +392,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <charset val="0"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -460,14 +465,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFE7E7E7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7E7E7"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -513,10 +518,10 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -545,8 +550,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
@@ -566,7 +571,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr/>
-  <dimension ref="A1:AMG31"/>
+  <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView defaultGridColor="0" colorId="64" view="normal" tabSelected="1" workbookViewId="0">
       <selection pane="topLeft" activeCell="AA11" sqref="AA11"/>
@@ -719,7 +724,7 @@
         <v>32</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -1727,8 +1732,8 @@
       <c r="U17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="V17" s="3" t="s">
-        <v>32</v>
+      <c r="V17" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:22">
@@ -1796,7 +1801,7 @@
         <v>69</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="48">
@@ -1860,7 +1865,7 @@
         <v>32</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:22">
@@ -1928,7 +1933,7 @@
         <v>32</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:22">
@@ -1996,7 +2001,7 @@
         <v>32</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="48">
@@ -2064,7 +2069,7 @@
         <v>32</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="48">
@@ -2132,7 +2137,7 @@
         <v>32</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="48">
@@ -2200,7 +2205,7 @@
         <v>32</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="48">
@@ -2268,7 +2273,7 @@
         <v>32</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="48">
@@ -2336,7 +2341,7 @@
         <v>32</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="48">
@@ -2404,7 +2409,7 @@
         <v>32</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="48">
@@ -2472,7 +2477,7 @@
         <v>32</v>
       </c>
       <c r="V28" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="48">
@@ -2540,7 +2545,7 @@
         <v>32</v>
       </c>
       <c r="V29" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="48">
@@ -2608,7 +2613,7 @@
         <v>32</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="48">
@@ -2676,7 +2681,7 @@
         <v>32</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
keyboard shortcuts keywords and test data
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/keyboard_shortcut_test_data.xlsx
+++ b/TestData/Web_POS/Billing/keyboard_shortcut_test_data.xlsx
@@ -60,6 +60,9 @@
     <t>buy_items</t>
   </si>
   <si>
+    <t>get_items</t>
+  </si>
+  <si>
     <t>dob</t>
   </si>
   <si>
@@ -87,6 +90,9 @@
     <t>shortcut_key</t>
   </si>
   <si>
+    <t>group</t>
+  </si>
+  <si>
     <t>KB_1</t>
   </si>
   <si>
@@ -138,6 +144,9 @@
     <t>KB_4</t>
   </si>
   <si>
+    <t>CTRL+1</t>
+  </si>
+  <si>
     <t>KB_5</t>
   </si>
   <si>
@@ -147,39 +156,78 @@
     <t>Amount : 10</t>
   </si>
   <si>
+    <t>CTRL+2</t>
+  </si>
+  <si>
     <t>KB_6</t>
   </si>
   <si>
     <t>cash : 100, paytm : 100, voucher : 0</t>
   </si>
   <si>
+    <t>CTRL+3</t>
+  </si>
+  <si>
     <t>KB_7</t>
   </si>
   <si>
+    <t>CTRL+5</t>
+  </si>
+  <si>
     <t>KB_8</t>
   </si>
   <si>
+    <t>Carry Bag Latest : 1</t>
+  </si>
+  <si>
+    <t>CTRL+6</t>
+  </si>
+  <si>
     <t>KB_9</t>
   </si>
   <si>
     <t>QBSB-Specificqty-Flat-rupees</t>
   </si>
   <si>
+    <t>CTRL+a</t>
+  </si>
+  <si>
     <t>KB_10</t>
   </si>
   <si>
     <t>KB_11</t>
   </si>
   <si>
+    <t>CTRL+x</t>
+  </si>
+  <si>
     <t>KB_12</t>
   </si>
   <si>
+    <t>CTRL+b</t>
+  </si>
+  <si>
     <t>KB_13</t>
   </si>
   <si>
+    <t>307260624Wa9</t>
+  </si>
+  <si>
+    <t>userone_p10</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
     <t>KB_14</t>
   </si>
   <si>
+    <t>307260624dq3</t>
+  </si>
+  <si>
+    <t>userone_p9</t>
+  </si>
+  <si>
     <t>KB_15</t>
   </si>
   <si>
@@ -192,19 +240,22 @@
     <t>Order</t>
   </si>
   <si>
+    <t>CTRL+s</t>
+  </si>
+  <si>
     <t>KB_17</t>
   </si>
   <si>
-    <t>MrunalJagtap</t>
-  </si>
-  <si>
-    <t>Rudraksha : 2, Carry bag : 1</t>
+    <t>CTRL+G</t>
   </si>
   <si>
     <t>KB_18</t>
   </si>
   <si>
     <t>QBSB-Specificity-Flat-fixed-all</t>
+  </si>
+  <si>
+    <t>CTRL+ALT+R</t>
   </si>
   <si>
     <t>KB_19</t>
@@ -663,8 +714,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="J1">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="K16">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -682,7 +733,12 @@
     <col min="11" max="11" width="18.20703" customWidth="1"/>
     <col min="12" max="12" width="20.17969" customWidth="1"/>
     <col min="13" max="13" width="21.85547" customWidth="1"/>
-    <col min="14" max="1020" width="11.42969" customWidth="1"/>
+    <col min="14" max="14" width="21.85547" customWidth="1"/>
+    <col min="15" max="20" width="11.42969" customWidth="1"/>
+    <col min="21" max="21" width="20.71094" customWidth="1"/>
+    <col min="22" max="22" width="11.42969" customWidth="1"/>
+    <col min="23" max="23" width="14.28516" customWidth="1"/>
+    <col min="24" max="1021" width="11.42969" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.5">
@@ -734,7 +790,7 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R1" s="3" t="s">
@@ -743,31 +799,37 @@
       <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1">
         <v>123456</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1">
         <v>123456</v>
@@ -779,61 +841,64 @@
         <v>600</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="3"/>
       <c r="S2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V2" t="s">
-        <v>30</v>
+      <c r="V2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1">
         <v>123456</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1">
         <v>123456</v>
@@ -845,61 +910,64 @@
         <v>600</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="3"/>
       <c r="S3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="V3" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" ht="28.5">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5">
         <v>123456</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F4" s="5">
         <v>123456</v>
@@ -911,10 +979,10 @@
         <v>600</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K4" s="6">
         <v>1</v>
@@ -923,49 +991,52 @@
         <v>2</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="8"/>
       <c r="P4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="V4" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" ht="28.5">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" s="5">
         <v>123456</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5">
         <v>123456</v>
@@ -977,10 +1048,10 @@
         <v>600</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K5" s="6">
         <v>1</v>
@@ -989,46 +1060,52 @@
         <v>2</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="8"/>
       <c r="P5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" ht="38.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2">
         <v>123456</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2">
         <v>123456</v>
@@ -1040,7 +1117,7 @@
         <v>600</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J6" s="9">
         <v>1</v>
@@ -1049,51 +1126,57 @@
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" s="10">
+        <v>30</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="10">
         <v>45384</v>
       </c>
-      <c r="O6" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" ht="25.5">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2">
         <v>123456</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2">
         <v>123456</v>
@@ -1105,7 +1188,7 @@
         <v>600</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J7" s="9">
         <v>1</v>
@@ -1114,51 +1197,57 @@
         <v>1</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N7" s="10">
+        <v>30</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="10">
         <v>45384</v>
       </c>
-      <c r="O7" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P7" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R7" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S7" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" ht="25.5">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2">
         <v>123456</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2">
         <v>123456</v>
@@ -1170,7 +1259,7 @@
         <v>600</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J8" s="9">
         <v>1</v>
@@ -1179,51 +1268,57 @@
         <v>1</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8" s="10">
+        <v>30</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" s="10">
         <v>45384</v>
       </c>
-      <c r="O8" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R8" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S8" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="9" ht="28.5">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D9" s="5">
         <v>123456</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F9" s="5">
         <v>123456</v>
@@ -1235,10 +1330,10 @@
         <v>600</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K9" s="6">
         <v>1</v>
@@ -1247,46 +1342,52 @@
         <v>2</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" s="8"/>
       <c r="P9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="11">
+        <v>7709577438</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>27</v>
+        <v>52</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5">
         <v>123456</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F10" s="5">
         <v>123456</v>
@@ -1298,10 +1399,10 @@
         <v>600</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="K10" s="6">
         <v>1</v>
@@ -1310,46 +1411,52 @@
         <v>2</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="8"/>
       <c r="P10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R10" s="11">
+        <v>7709577438</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" ht="25.5">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2">
         <v>123456</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2">
         <v>123456</v>
@@ -1361,7 +1468,7 @@
         <v>600</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J11" s="9">
         <v>1</v>
@@ -1370,51 +1477,57 @@
         <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N11" s="10">
+        <v>30</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="10">
         <v>45384</v>
       </c>
-      <c r="O11" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q11" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R11" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" ht="25.5">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2">
         <v>123456</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F12" s="2">
         <v>123456</v>
@@ -1426,7 +1539,7 @@
         <v>600</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J12" s="9">
         <v>1</v>
@@ -1435,51 +1548,57 @@
         <v>1</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" s="10">
+        <v>30</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="10">
         <v>45384</v>
       </c>
-      <c r="O12" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q12" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R12" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R12" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S12" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" ht="25.5">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2">
         <v>123456</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F13" s="2">
         <v>123456</v>
@@ -1491,7 +1610,7 @@
         <v>600</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J13" s="9">
         <v>1</v>
@@ -1500,51 +1619,57 @@
         <v>1</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N13" s="10">
+        <v>30</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" s="10">
         <v>45384</v>
       </c>
-      <c r="O13" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P13" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q13" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R13" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R13" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W13" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" ht="25.5">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2">
         <v>123456</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="F14" s="2">
         <v>123456</v>
@@ -1556,7 +1681,7 @@
         <v>600</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J14" s="9">
         <v>1</v>
@@ -1565,51 +1690,60 @@
         <v>1</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="10">
+        <v>30</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" s="10">
         <v>45384</v>
       </c>
-      <c r="O14" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q14" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R14" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R14" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S14" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W14" t="s">
+        <v>61</v>
+      </c>
+      <c r="X14" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="15" ht="25.5">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D15" s="12">
         <v>123456</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="F15" s="2">
         <v>123456</v>
@@ -1621,7 +1755,7 @@
         <v>600</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J15" s="9">
         <v>1</v>
@@ -1630,51 +1764,57 @@
         <v>1</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N15" s="10">
+        <v>30</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" s="10">
         <v>45384</v>
       </c>
-      <c r="O15" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q15" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R15" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R15" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S15" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W15" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5">
         <v>123456</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F16" s="5">
         <v>123456</v>
@@ -1683,13 +1823,13 @@
         <v>1000</v>
       </c>
       <c r="H16" s="6">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="K16" s="6">
         <v>1</v>
@@ -1698,46 +1838,52 @@
         <v>1</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" s="8"/>
       <c r="P16" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R16" s="11">
+        <v>7709577438</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W16" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="17" ht="38.25">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2">
         <v>123456</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F17" s="2">
         <v>123456</v>
@@ -1749,7 +1895,7 @@
         <v>600</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J17" s="9">
         <v>1</v>
@@ -1758,51 +1904,57 @@
         <v>1</v>
       </c>
       <c r="L17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O17" s="10">
+        <v>45384</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17" s="11">
+        <v>7709577438</v>
+      </c>
+      <c r="S17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N17" s="10">
-        <v>45384</v>
-      </c>
-      <c r="O17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="P17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q17" s="11">
-        <v>7709577438</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="T17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W17" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D18" s="13">
         <v>123456</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>58</v>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="F18" s="1">
         <v>123456</v>
@@ -1814,60 +1966,66 @@
         <v>600</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R18" s="11">
+        <v>7709577438</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W18" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D19" s="5">
         <v>123456</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F19" s="5">
         <v>123456</v>
@@ -1879,10 +2037,10 @@
         <v>600</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="K19" s="6">
         <v>1</v>
@@ -1891,44 +2049,50 @@
         <v>1</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O19" s="8"/>
       <c r="P19" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R19" s="11">
+        <v>7709577438</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W19" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1">
         <v>123456</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F20" s="1">
         <v>123456</v>
@@ -1940,60 +2104,66 @@
         <v>600</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R20" s="11">
+        <v>7709577438</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1">
         <v>123456</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F21" s="1">
         <v>123456</v>
@@ -2005,60 +2175,66 @@
         <v>600</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N21" s="14">
+        <v>30</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O21" s="14">
         <v>45384</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S21" s="3">
+        <v>37</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R21" s="11">
+        <v>7709577438</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T21" s="3">
         <v>300</v>
       </c>
-      <c r="T21" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="U21" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W21" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22" ht="25.5">
       <c r="A22" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D22" s="2">
         <v>123456</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F22" s="2">
         <v>123456</v>
@@ -2070,7 +2246,7 @@
         <v>600</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J22" s="9">
         <v>1</v>
@@ -2079,51 +2255,57 @@
         <v>1</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N22" s="10">
+        <v>30</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O22" s="10">
         <v>45384</v>
       </c>
-      <c r="O22" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q22" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R22" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R22" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W22" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" ht="25.5">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D23" s="2">
         <v>123456</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F23" s="2">
         <v>123456</v>
@@ -2135,7 +2317,7 @@
         <v>600</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J23" s="9">
         <v>1</v>
@@ -2144,51 +2326,57 @@
         <v>1</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N23" s="10">
+        <v>30</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O23" s="10">
         <v>45384</v>
       </c>
-      <c r="O23" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P23" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q23" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R23" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R23" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W23" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" ht="25.5">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D24" s="2">
         <v>123456</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F24" s="2">
         <v>123456</v>
@@ -2200,7 +2388,7 @@
         <v>600</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J24" s="9">
         <v>1</v>
@@ -2209,51 +2397,57 @@
         <v>1</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N24" s="10">
+        <v>30</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O24" s="10">
         <v>45384</v>
       </c>
-      <c r="O24" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P24" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q24" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R24" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R24" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T24" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W24" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" ht="25.5">
       <c r="A25" s="1" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D25" s="2">
         <v>123456</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F25" s="2">
         <v>123456</v>
@@ -2265,7 +2459,7 @@
         <v>600</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J25" s="9">
         <v>1</v>
@@ -2274,51 +2468,54 @@
         <v>1</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N25" s="10">
+        <v>30</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O25" s="10">
         <v>45384</v>
       </c>
-      <c r="O25" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P25" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q25" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R25" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R25" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T25" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="26" ht="25.5">
       <c r="A26" s="1" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D26" s="2">
         <v>123456</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F26" s="2">
         <v>123456</v>
@@ -2330,7 +2527,7 @@
         <v>600</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J26" s="9">
         <v>1</v>
@@ -2339,51 +2536,54 @@
         <v>1</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N26" s="10">
+        <v>30</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O26" s="10">
         <v>45384</v>
       </c>
-      <c r="O26" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P26" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q26" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R26" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R26" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="27" ht="25.5">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D27" s="2">
         <v>123456</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F27" s="2">
         <v>123456</v>
@@ -2395,7 +2595,7 @@
         <v>600</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J27" s="9">
         <v>1</v>
@@ -2404,51 +2604,54 @@
         <v>1</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N27" s="10">
+        <v>30</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O27" s="10">
         <v>45384</v>
       </c>
-      <c r="O27" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P27" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q27" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R27" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R27" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="28" ht="25.5">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D28" s="2">
         <v>123456</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F28" s="2">
         <v>123456</v>
@@ -2460,7 +2663,7 @@
         <v>600</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J28" s="9">
         <v>1</v>
@@ -2469,51 +2672,54 @@
         <v>1</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N28" s="10">
+        <v>30</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O28" s="10">
         <v>45384</v>
       </c>
-      <c r="O28" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P28" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q28" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R28" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R28" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T28" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="29" ht="25.5">
       <c r="A29" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D29" s="2">
         <v>123456</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F29" s="2">
         <v>123456</v>
@@ -2525,7 +2731,7 @@
         <v>600</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J29" s="9">
         <v>1</v>
@@ -2534,51 +2740,54 @@
         <v>1</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N29" s="10">
+        <v>30</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O29" s="10">
         <v>45384</v>
       </c>
-      <c r="O29" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P29" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q29" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R29" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R29" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="30" ht="25.5">
       <c r="A30" s="1" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D30" s="2">
         <v>123456</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F30" s="2">
         <v>123456</v>
@@ -2590,7 +2799,7 @@
         <v>600</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J30" s="9">
         <v>1</v>
@@ -2599,51 +2808,54 @@
         <v>1</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N30" s="10">
+        <v>30</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O30" s="10">
         <v>45384</v>
       </c>
-      <c r="O30" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P30" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q30" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q30" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R30" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R30" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T30" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="31" ht="25.5">
       <c r="A31" s="1" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D31" s="2">
         <v>123456</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F31" s="2">
         <v>123456</v>
@@ -2655,7 +2867,7 @@
         <v>600</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J31" s="9">
         <v>1</v>
@@ -2664,34 +2876,37 @@
         <v>1</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N31" s="10">
+        <v>30</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O31" s="10">
         <v>45384</v>
       </c>
-      <c r="O31" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="P31" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q31" s="11">
+        <v>37</v>
+      </c>
+      <c r="Q31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="R31" s="11">
         <v>7709577438</v>
       </c>
-      <c r="R31" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="S31" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="T31" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>73</v>
+        <v>29</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>